<commit_message>
updated hull to hull v2. should be more hydrodynamic..
improvements on form could still be made
</commit_message>
<xml_diff>
--- a/mechanical/SolidWorks/Prototype/airfoil coords.xlsx
+++ b/mechanical/SolidWorks/Prototype/airfoil coords.xlsx
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>